<commit_message>
Update slides and data 2021-1
</commit_message>
<xml_diff>
--- a/004_1.1.1.EMP_Total_nacional_IQY.xlsx
+++ b/004_1.1.1.EMP_Total_nacional_IQY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
     <t>Tasas de empleo y desempleo - Porcentaje de fuerza de trabajo</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t>Tasa de desempleo (%)</t>
+  </si>
+  <si>
+    <t>2020-12</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>2020-10</t>
+  </si>
+  <si>
+    <t>2020-09</t>
+  </si>
+  <si>
+    <t>2020-08</t>
+  </si>
+  <si>
+    <t>2020-07</t>
   </si>
   <si>
     <t>2020-06</t>
@@ -1352,7 +1370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D263"/>
+  <dimension ref="A1:D269"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,10 +1441,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="11">
-        <v>46.0522138627812</v>
+        <v>53.4110282760894</v>
       </c>
       <c r="C10" s="12">
-        <v>19.8131768373933</v>
+        <v>13.3717176087206</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.06" customHeight="1">
@@ -1434,10 +1452,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="14">
-        <v>43.3808099067874</v>
+        <v>53.225283173092</v>
       </c>
       <c r="C11" s="15">
-        <v>21.3784917915415</v>
+        <v>13.3111917867181</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.06" customHeight="1">
@@ -1445,10 +1463,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="11">
-        <v>41.5703596167582</v>
+        <v>53.1852823609757</v>
       </c>
       <c r="C12" s="12">
-        <v>19.8111421208653</v>
+        <v>14.6507309342331</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.06" customHeight="1">
@@ -1456,10 +1474,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="14">
-        <v>51.7022872235407</v>
+        <v>50.6310960429763</v>
       </c>
       <c r="C13" s="15">
-        <v>12.6341056681643</v>
+        <v>15.7710538674914</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.06" customHeight="1">
@@ -1467,10 +1485,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="11">
-        <v>55.4755307491681</v>
+        <v>49.3440046062558</v>
       </c>
       <c r="C14" s="12">
-        <v>12.1552632018055</v>
+        <v>16.75725761208</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.06" customHeight="1">
@@ -1478,10 +1496,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="14">
-        <v>54.3706724439715</v>
+        <v>45.098526066259</v>
       </c>
       <c r="C15" s="15">
-        <v>12.9879981543389</v>
+        <v>20.2235286868572</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.06" customHeight="1">
@@ -1489,10 +1507,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="11">
-        <v>57.4995892927981</v>
+        <v>46.0522138627812</v>
       </c>
       <c r="C16" s="12">
-        <v>9.53174880650129</v>
+        <v>19.8131768373933</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.06" customHeight="1">
@@ -1500,10 +1518,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="14">
-        <v>57.8477927848472</v>
+        <v>43.3808099067874</v>
       </c>
       <c r="C17" s="15">
-        <v>9.25094900998434</v>
+        <v>21.3784917915415</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.06" customHeight="1">
@@ -1511,10 +1529,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="11">
-        <v>57.7539064665701</v>
+        <v>41.5703596167582</v>
       </c>
       <c r="C18" s="12">
-        <v>9.84162483290371</v>
+        <v>19.8111421208653</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.06" customHeight="1">
@@ -1522,10 +1540,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="14">
-        <v>56.3356438857068</v>
+        <v>51.7022872235407</v>
       </c>
       <c r="C19" s="15">
-        <v>10.2237111384426</v>
+        <v>12.6341056681643</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.06" customHeight="1">
@@ -1533,10 +1551,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="11">
-        <v>56.1070602967198</v>
+        <v>55.4755307491681</v>
       </c>
       <c r="C20" s="12">
-        <v>10.7963281082675</v>
+        <v>12.1552632018055</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.06" customHeight="1">
@@ -1544,10 +1562,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="14">
-        <v>56.2274513984853</v>
+        <v>54.3706724439715</v>
       </c>
       <c r="C21" s="15">
-        <v>10.7160765202848</v>
+        <v>12.9879981543389</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.06" customHeight="1">
@@ -1555,10 +1573,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="11">
-        <v>57.502365627045</v>
+        <v>57.4995892927981</v>
       </c>
       <c r="C22" s="12">
-        <v>9.43709347095469</v>
+        <v>9.53174880650129</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.06" customHeight="1">
@@ -1566,10 +1584,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="14">
-        <v>56.4082388013268</v>
+        <v>57.8477927848472</v>
       </c>
       <c r="C23" s="15">
-        <v>10.5376432538346</v>
+        <v>9.25094900998434</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.06" customHeight="1">
@@ -1577,10 +1595,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="11">
-        <v>55.7847794572863</v>
+        <v>57.7539064665701</v>
       </c>
       <c r="C24" s="12">
-        <v>10.3343428077985</v>
+        <v>9.84162483290371</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.06" customHeight="1">
@@ -1588,10 +1606,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="14">
-        <v>56.3933356269048</v>
+        <v>56.3356438857068</v>
       </c>
       <c r="C25" s="15">
-        <v>10.8165675901179</v>
+        <v>10.2237111384426</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.06" customHeight="1">
@@ -1599,10 +1617,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="11">
-        <v>56.3505119490261</v>
+        <v>56.1070602967198</v>
       </c>
       <c r="C26" s="12">
-        <v>11.7683980121889</v>
+        <v>10.7963281082675</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.06" customHeight="1">
@@ -1610,10 +1628,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="14">
-        <v>55.3335593546967</v>
+        <v>56.2274513984853</v>
       </c>
       <c r="C27" s="15">
-        <v>12.7954576332439</v>
+        <v>10.7160765202848</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.06" customHeight="1">
@@ -1621,10 +1639,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="11">
-        <v>58.7267215244695</v>
+        <v>57.502365627045</v>
       </c>
       <c r="C28" s="12">
-        <v>9.72109011461203</v>
+        <v>9.43709347095469</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.06" customHeight="1">
@@ -1632,10 +1650,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="14">
-        <v>57.530724382807</v>
+        <v>56.4082388013268</v>
       </c>
       <c r="C29" s="15">
-        <v>8.75834591165997</v>
+        <v>10.5376432538346</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.06" customHeight="1">
@@ -1643,10 +1661,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="11">
-        <v>59.2238163143154</v>
+        <v>55.7847794572863</v>
       </c>
       <c r="C30" s="12">
-        <v>9.06119915105479</v>
+        <v>10.3343428077985</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.06" customHeight="1">
@@ -1654,10 +1672,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="14">
-        <v>58.2753169073156</v>
+        <v>56.3933356269048</v>
       </c>
       <c r="C31" s="15">
-        <v>9.48218505837844</v>
+        <v>10.8165675901179</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.06" customHeight="1">
@@ -1665,10 +1683,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="11">
-        <v>58.2714716920938</v>
+        <v>56.3505119490261</v>
       </c>
       <c r="C32" s="12">
-        <v>9.15641456632453</v>
+        <v>11.7683980121889</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.06" customHeight="1">
@@ -1676,10 +1694,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="14">
-        <v>57.4403226513407</v>
+        <v>55.3335593546967</v>
       </c>
       <c r="C33" s="15">
-        <v>9.72066629402551</v>
+        <v>12.7954576332439</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.06" customHeight="1">
@@ -1687,10 +1705,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="11">
-        <v>58.3104440454891</v>
+        <v>58.7267215244695</v>
       </c>
       <c r="C34" s="12">
-        <v>9.08208673816314</v>
+        <v>9.72109011461203</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.06" customHeight="1">
@@ -1698,10 +1716,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="14">
-        <v>57.874215708365</v>
+        <v>57.530724382807</v>
       </c>
       <c r="C35" s="15">
-        <v>9.72997338525743</v>
+        <v>8.75834591165997</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.06" customHeight="1">
@@ -1709,10 +1727,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="11">
-        <v>58.5039801578665</v>
+        <v>59.2238163143154</v>
       </c>
       <c r="C36" s="12">
-        <v>9.46258583543159</v>
+        <v>9.06119915105479</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.06" customHeight="1">
@@ -1720,10 +1738,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="14">
-        <v>56.9939904899045</v>
+        <v>58.2753169073156</v>
       </c>
       <c r="C37" s="15">
-        <v>9.43596717337635</v>
+        <v>9.48218505837844</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.06" customHeight="1">
@@ -1731,10 +1749,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="11">
-        <v>56.4798613555524</v>
+        <v>58.2714716920938</v>
       </c>
       <c r="C38" s="12">
-        <v>10.8032182510231</v>
+        <v>9.15641456632453</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.06" customHeight="1">
@@ -1742,10 +1760,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="14">
-        <v>55.8013048579568</v>
+        <v>57.4403226513407</v>
       </c>
       <c r="C39" s="15">
-        <v>11.7623483380153</v>
+        <v>9.72066629402551</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.06" customHeight="1">
@@ -1753,10 +1771,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="11">
-        <v>58.7000452147639</v>
+        <v>58.3104440454891</v>
       </c>
       <c r="C40" s="12">
-        <v>8.62738893216062</v>
+        <v>9.08208673816314</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.06" customHeight="1">
@@ -1764,10 +1782,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="14">
-        <v>59.3450920091798</v>
+        <v>57.874215708365</v>
       </c>
       <c r="C41" s="15">
-        <v>8.37056422532671</v>
+        <v>9.72997338525743</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.06" customHeight="1">
@@ -1775,10 +1793,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="11">
-        <v>59.9502250185514</v>
+        <v>58.5039801578665</v>
       </c>
       <c r="C42" s="12">
-        <v>8.55558571797357</v>
+        <v>9.46258583543159</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.06" customHeight="1">
@@ -1786,10 +1804,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="14">
-        <v>58.2356564083588</v>
+        <v>56.9939904899045</v>
       </c>
       <c r="C43" s="15">
-        <v>9.2246951183925</v>
+        <v>9.43596717337635</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.06" customHeight="1">
@@ -1797,10 +1815,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="11">
-        <v>58.6131205052832</v>
+        <v>56.4798613555524</v>
       </c>
       <c r="C44" s="12">
-        <v>9.10041094030727</v>
+        <v>10.8032182510231</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.06" customHeight="1">
@@ -1808,10 +1826,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="14">
-        <v>57.5184270279998</v>
+        <v>55.8013048579568</v>
       </c>
       <c r="C45" s="15">
-        <v>9.67541135213215</v>
+        <v>11.7623483380153</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.06" customHeight="1">
@@ -1819,10 +1837,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="11">
-        <v>59.4843458883889</v>
+        <v>58.7000452147639</v>
       </c>
       <c r="C46" s="12">
-        <v>8.71552219742322</v>
+        <v>8.62738893216062</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.06" customHeight="1">
@@ -1830,10 +1848,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="14">
-        <v>58.1394250189673</v>
+        <v>59.3450920091798</v>
       </c>
       <c r="C47" s="15">
-        <v>9.41700074743494</v>
+        <v>8.37056422532671</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.06" customHeight="1">
@@ -1841,10 +1859,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="11">
-        <v>59.2639485287101</v>
+        <v>59.9502250185514</v>
       </c>
       <c r="C48" s="12">
-        <v>8.90771809538689</v>
+        <v>8.55558571797357</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.06" customHeight="1">
@@ -1852,10 +1870,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="14">
-        <v>57.401697325841</v>
+        <v>58.2356564083588</v>
       </c>
       <c r="C49" s="15">
-        <v>9.70461035985844</v>
+        <v>9.2246951183925</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.06" customHeight="1">
@@ -1863,10 +1881,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="11">
-        <v>57.2509458052721</v>
+        <v>58.6131205052832</v>
       </c>
       <c r="C50" s="12">
-        <v>10.504291994031</v>
+        <v>9.10041094030727</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.06" customHeight="1">
@@ -1874,10 +1892,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="14">
-        <v>56.3435634077781</v>
+        <v>57.5184270279998</v>
       </c>
       <c r="C51" s="15">
-        <v>11.7332667441449</v>
+        <v>9.67541135213215</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.06" customHeight="1">
@@ -1885,10 +1903,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="11">
-        <v>58.9793736870061</v>
+        <v>59.4843458883889</v>
       </c>
       <c r="C52" s="12">
-        <v>8.74275606903631</v>
+        <v>8.71552219742322</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.06" customHeight="1">
@@ -1896,10 +1914,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="14">
-        <v>60.3461237428842</v>
+        <v>58.1394250189673</v>
       </c>
       <c r="C53" s="15">
-        <v>7.50942303985622</v>
+        <v>9.41700074743494</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.06" customHeight="1">
@@ -1907,10 +1925,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="11">
-        <v>60.7713373129316</v>
+        <v>59.2639485287101</v>
       </c>
       <c r="C54" s="12">
-        <v>8.29432074855555</v>
+        <v>8.90771809538689</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.06" customHeight="1">
@@ -1918,10 +1936,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="14">
-        <v>58.7147551995271</v>
+        <v>57.401697325841</v>
       </c>
       <c r="C55" s="15">
-        <v>8.50788441336333</v>
+        <v>9.70461035985844</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.06" customHeight="1">
@@ -1929,10 +1947,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="11">
-        <v>58.7887608310492</v>
+        <v>57.2509458052721</v>
       </c>
       <c r="C56" s="12">
-        <v>8.98841963883306</v>
+        <v>10.504291994031</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.06" customHeight="1">
@@ -1940,10 +1958,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="14">
-        <v>57.2982272857362</v>
+        <v>56.3435634077781</v>
       </c>
       <c r="C57" s="15">
-        <v>9.84530811145194</v>
+        <v>11.7332667441449</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.06" customHeight="1">
@@ -1951,10 +1969,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="11">
-        <v>58.8172072514158</v>
+        <v>58.9793736870061</v>
       </c>
       <c r="C58" s="12">
-        <v>8.88315837113411</v>
+        <v>8.74275606903631</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.06" customHeight="1">
@@ -1962,10 +1980,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="14">
-        <v>58.2208299290644</v>
+        <v>60.3461237428842</v>
       </c>
       <c r="C59" s="15">
-        <v>8.84744743913623</v>
+        <v>7.50942303985622</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.06" customHeight="1">
@@ -1973,10 +1991,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="11">
-        <v>58.7595506115685</v>
+        <v>60.7713373129316</v>
       </c>
       <c r="C60" s="12">
-        <v>9.01580783936775</v>
+        <v>8.29432074855555</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.06" customHeight="1">
@@ -1984,10 +2002,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="14">
-        <v>56.8817469810815</v>
+        <v>58.7147551995271</v>
       </c>
       <c r="C61" s="15">
-        <v>10.1373919332206</v>
+        <v>8.50788441336333</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.06" customHeight="1">
@@ -1995,10 +2013,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="11">
-        <v>57.9335833137289</v>
+        <v>58.7887608310492</v>
       </c>
       <c r="C62" s="12">
-        <v>10.0025396274902</v>
+        <v>8.98841963883306</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.06" customHeight="1">
@@ -2006,10 +2024,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="14">
-        <v>56.8634259649992</v>
+        <v>57.2982272857362</v>
       </c>
       <c r="C63" s="15">
-        <v>11.9053301165896</v>
+        <v>9.84530811145194</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.06" customHeight="1">
@@ -2017,10 +2035,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="11">
-        <v>59.5244924400714</v>
+        <v>58.8172072514158</v>
       </c>
       <c r="C64" s="12">
-        <v>8.5889170899724</v>
+        <v>8.88315837113411</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.06" customHeight="1">
@@ -2028,10 +2046,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="14">
-        <v>60.8756551505599</v>
+        <v>58.2208299290644</v>
       </c>
       <c r="C65" s="15">
-        <v>7.27097077778655</v>
+        <v>8.84744743913623</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.06" customHeight="1">
@@ -2039,10 +2057,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="11">
-        <v>61.4105913604164</v>
+        <v>58.7595506115685</v>
       </c>
       <c r="C66" s="12">
-        <v>8.18502461480289</v>
+        <v>9.01580783936775</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.06" customHeight="1">
@@ -2050,10 +2068,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="14">
-        <v>58.7146237165434</v>
+        <v>56.8817469810815</v>
       </c>
       <c r="C67" s="15">
-        <v>8.98076767370366</v>
+        <v>10.1373919332206</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.06" customHeight="1">
@@ -2061,10 +2079,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="11">
-        <v>58.8605007750852</v>
+        <v>57.9335833137289</v>
       </c>
       <c r="C68" s="12">
-        <v>9.09395685250873</v>
+        <v>10.0025396274902</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.06" customHeight="1">
@@ -2072,10 +2090,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="14">
-        <v>58.3520587082019</v>
+        <v>56.8634259649992</v>
       </c>
       <c r="C69" s="15">
-        <v>8.83940166273367</v>
+        <v>11.9053301165896</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.06" customHeight="1">
@@ -2083,10 +2101,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="11">
-        <v>59.0984527642152</v>
+        <v>59.5244924400714</v>
       </c>
       <c r="C70" s="12">
-        <v>8.24578793685616</v>
+        <v>8.5889170899724</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.06" customHeight="1">
@@ -2094,10 +2112,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="14">
-        <v>58.8136448755721</v>
+        <v>60.8756551505599</v>
       </c>
       <c r="C71" s="15">
-        <v>8.9337302074684</v>
+        <v>7.27097077778655</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.06" customHeight="1">
@@ -2105,10 +2123,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="11">
-        <v>59.2722002138265</v>
+        <v>61.4105913604164</v>
       </c>
       <c r="C72" s="12">
-        <v>9.50407118412518</v>
+        <v>8.18502461480289</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.06" customHeight="1">
@@ -2116,10 +2134,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="14">
-        <v>58.2300302248588</v>
+        <v>58.7146237165434</v>
       </c>
       <c r="C73" s="15">
-        <v>8.86061044787356</v>
+        <v>8.98076767370366</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.06" customHeight="1">
@@ -2127,10 +2145,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="11">
-        <v>57.3897297413554</v>
+        <v>58.8605007750852</v>
       </c>
       <c r="C74" s="12">
-        <v>9.85631634014762</v>
+        <v>9.09395685250873</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.06" customHeight="1">
@@ -2138,10 +2156,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="14">
-        <v>56.9353490687088</v>
+        <v>58.3520587082019</v>
       </c>
       <c r="C75" s="15">
-        <v>10.7851505845238</v>
+        <v>8.83940166273367</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.06" customHeight="1">
@@ -2149,10 +2167,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="11">
-        <v>58.8793176667615</v>
+        <v>59.0984527642152</v>
       </c>
       <c r="C76" s="12">
-        <v>8.72291410603385</v>
+        <v>8.24578793685616</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.06" customHeight="1">
@@ -2160,10 +2178,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="14">
-        <v>60.3334479536757</v>
+        <v>58.8136448755721</v>
       </c>
       <c r="C77" s="15">
-        <v>7.71001420344498</v>
+        <v>8.9337302074684</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.06" customHeight="1">
@@ -2171,10 +2189,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="11">
-        <v>61.274883625071</v>
+        <v>59.2722002138265</v>
       </c>
       <c r="C78" s="12">
-        <v>7.86026383778776</v>
+        <v>9.50407118412518</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.06" customHeight="1">
@@ -2182,10 +2200,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="14">
-        <v>59.1562236831617</v>
+        <v>58.2300302248588</v>
       </c>
       <c r="C79" s="15">
-        <v>8.3503507604119</v>
+        <v>8.86061044787356</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.06" customHeight="1">
@@ -2193,10 +2211,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="11">
-        <v>58.9705292983714</v>
+        <v>57.3897297413554</v>
       </c>
       <c r="C80" s="12">
-        <v>8.90102748373475</v>
+        <v>9.85631634014762</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.06" customHeight="1">
@@ -2204,10 +2222,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="14">
-        <v>57.6436476583292</v>
+        <v>56.9353490687088</v>
       </c>
       <c r="C81" s="15">
-        <v>9.28975314197442</v>
+        <v>10.7851505845238</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.06" customHeight="1">
@@ -2215,10 +2233,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="11">
-        <v>58.348408500593</v>
+        <v>58.8793176667615</v>
       </c>
       <c r="C82" s="12">
-        <v>9.19461358146464</v>
+        <v>8.72291410603385</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.06" customHeight="1">
@@ -2226,10 +2244,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="14">
-        <v>58.322946414215</v>
+        <v>60.3334479536757</v>
       </c>
       <c r="C83" s="15">
-        <v>8.79823689095793</v>
+        <v>7.71001420344498</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.06" customHeight="1">
@@ -2237,10 +2255,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="11">
-        <v>58.1249392167846</v>
+        <v>61.274883625071</v>
       </c>
       <c r="C84" s="12">
-        <v>8.96500304016321</v>
+        <v>7.86026383778776</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15.06" customHeight="1">
@@ -2248,10 +2266,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="14">
-        <v>56.7230007587655</v>
+        <v>59.1562236831617</v>
       </c>
       <c r="C85" s="15">
-        <v>9.73435127249192</v>
+        <v>8.3503507604119</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.06" customHeight="1">
@@ -2259,10 +2277,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="11">
-        <v>56.2917698513488</v>
+        <v>58.9705292983714</v>
       </c>
       <c r="C86" s="12">
-        <v>10.6791105334136</v>
+        <v>8.90102748373475</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.06" customHeight="1">
@@ -2270,10 +2288,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="14">
-        <v>56.562577636314</v>
+        <v>57.6436476583292</v>
       </c>
       <c r="C87" s="15">
-        <v>11.1012332832703</v>
+        <v>9.28975314197442</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.06" customHeight="1">
@@ -2281,10 +2299,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="11">
-        <v>59.0597481188486</v>
+        <v>58.348408500593</v>
       </c>
       <c r="C88" s="12">
-        <v>8.44215865502575</v>
+        <v>9.19461358146464</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.06" customHeight="1">
@@ -2292,10 +2310,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="14">
-        <v>58.8419078074567</v>
+        <v>58.322946414215</v>
       </c>
       <c r="C89" s="15">
-        <v>8.47943721306648</v>
+        <v>8.79823689095793</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.06" customHeight="1">
@@ -2303,10 +2321,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="11">
-        <v>60.9219664213861</v>
+        <v>58.1249392167846</v>
       </c>
       <c r="C90" s="12">
-        <v>7.79277690180104</v>
+        <v>8.96500304016321</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.06" customHeight="1">
@@ -2314,10 +2332,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="14">
-        <v>58.0060054604182</v>
+        <v>56.7230007587655</v>
       </c>
       <c r="C91" s="15">
-        <v>8.97842951018059</v>
+        <v>9.73435127249192</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.06" customHeight="1">
@@ -2325,10 +2343,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="11">
-        <v>58.5902438993544</v>
+        <v>56.2917698513488</v>
       </c>
       <c r="C92" s="12">
-        <v>9.26882643821622</v>
+        <v>10.6791105334136</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.06" customHeight="1">
@@ -2336,10 +2354,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="14">
-        <v>57.8077735732905</v>
+        <v>56.562577636314</v>
       </c>
       <c r="C93" s="15">
-        <v>9.88171557368344</v>
+        <v>11.1012332832703</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.06" customHeight="1">
@@ -2347,10 +2365,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="11">
-        <v>57.8426737418169</v>
+        <v>59.0597481188486</v>
       </c>
       <c r="C94" s="12">
-        <v>9.23667812796902</v>
+        <v>8.44215865502575</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.06" customHeight="1">
@@ -2358,10 +2376,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="14">
-        <v>58.7289380861254</v>
+        <v>58.8419078074567</v>
       </c>
       <c r="C95" s="15">
-        <v>9.4211416354269</v>
+        <v>8.47943721306648</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.06" customHeight="1">
@@ -2369,10 +2387,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="11">
-        <v>57.0006452841629</v>
+        <v>60.9219664213861</v>
       </c>
       <c r="C96" s="12">
-        <v>10.1736714086952</v>
+        <v>7.79277690180104</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.06" customHeight="1">
@@ -2380,10 +2398,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="14">
-        <v>56.470201755009</v>
+        <v>58.0060054604182</v>
       </c>
       <c r="C97" s="15">
-        <v>10.2061950614975</v>
+        <v>8.97842951018059</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.06" customHeight="1">
@@ -2391,10 +2409,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="11">
-        <v>56.1973408570218</v>
+        <v>58.5902438993544</v>
       </c>
       <c r="C98" s="12">
-        <v>11.7893105829725</v>
+        <v>9.26882643821622</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.06" customHeight="1">
@@ -2402,10 +2420,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="14">
-        <v>56.1585505702066</v>
+        <v>57.8077735732905</v>
       </c>
       <c r="C99" s="15">
-        <v>12.0697898274764</v>
+        <v>9.88171557368344</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.06" customHeight="1">
@@ -2413,10 +2431,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="11">
-        <v>58.4080203151737</v>
+        <v>57.8426737418169</v>
       </c>
       <c r="C100" s="12">
-        <v>9.55082463044959</v>
+        <v>9.23667812796902</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.06" customHeight="1">
@@ -2424,10 +2442,10 @@
         <v>99</v>
       </c>
       <c r="B101" s="14">
-        <v>58.3608315491595</v>
+        <v>58.7289380861254</v>
       </c>
       <c r="C101" s="15">
-        <v>9.24779272050277</v>
+        <v>9.4211416354269</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.06" customHeight="1">
@@ -2435,10 +2453,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="11">
-        <v>59.9361326157494</v>
+        <v>57.0006452841629</v>
       </c>
       <c r="C102" s="12">
-        <v>8.8534533595397</v>
+        <v>10.1736714086952</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.06" customHeight="1">
@@ -2446,10 +2464,10 @@
         <v>101</v>
       </c>
       <c r="B103" s="14">
-        <v>57.2710280842535</v>
+        <v>56.470201755009</v>
       </c>
       <c r="C103" s="15">
-        <v>9.94217224513115</v>
+        <v>10.2061950614975</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.06" customHeight="1">
@@ -2457,10 +2475,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="11">
-        <v>58.1399519609082</v>
+        <v>56.1973408570218</v>
       </c>
       <c r="C104" s="12">
-        <v>9.74827368704211</v>
+        <v>11.7893105829725</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.06" customHeight="1">
@@ -2468,10 +2486,10 @@
         <v>103</v>
       </c>
       <c r="B105" s="14">
-        <v>57.2153183174452</v>
+        <v>56.1585505702066</v>
       </c>
       <c r="C105" s="15">
-        <v>10.8630801444586</v>
+        <v>12.0697898274764</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.06" customHeight="1">
@@ -2479,10 +2497,10 @@
         <v>104</v>
       </c>
       <c r="B106" s="11">
-        <v>58.7882489224903</v>
+        <v>58.4080203151737</v>
       </c>
       <c r="C106" s="12">
-        <v>10.0261430976688</v>
+        <v>9.55082463044959</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.06" customHeight="1">
@@ -2490,10 +2508,10 @@
         <v>105</v>
       </c>
       <c r="B107" s="14">
-        <v>58.2579344584315</v>
+        <v>58.3608315491595</v>
       </c>
       <c r="C107" s="15">
-        <v>10.7094687859766</v>
+        <v>9.24779272050277</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.06" customHeight="1">
@@ -2501,10 +2519,10 @@
         <v>106</v>
       </c>
       <c r="B108" s="11">
-        <v>57.4815636439715</v>
+        <v>59.9361326157494</v>
       </c>
       <c r="C108" s="12">
-        <v>10.8641973805909</v>
+        <v>8.8534533595397</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.06" customHeight="1">
@@ -2512,10 +2530,10 @@
         <v>107</v>
       </c>
       <c r="B109" s="14">
-        <v>57.5243123196594</v>
+        <v>57.2710280842535</v>
       </c>
       <c r="C109" s="15">
-        <v>10.3637108530843</v>
+        <v>9.94217224513115</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.06" customHeight="1">
@@ -2523,10 +2541,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="11">
-        <v>56.7335788557677</v>
+        <v>58.1399519609082</v>
       </c>
       <c r="C110" s="12">
-        <v>11.869993035915</v>
+        <v>9.74827368704211</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.06" customHeight="1">
@@ -2534,10 +2552,10 @@
         <v>109</v>
       </c>
       <c r="B111" s="14">
-        <v>55.9507504385022</v>
+        <v>57.2153183174452</v>
       </c>
       <c r="C111" s="15">
-        <v>12.476696630348</v>
+        <v>10.8630801444586</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.06" customHeight="1">
@@ -2545,10 +2563,10 @@
         <v>110</v>
       </c>
       <c r="B112" s="11">
-        <v>58.5183522495253</v>
+        <v>58.7882489224903</v>
       </c>
       <c r="C112" s="12">
-        <v>9.8175710625056</v>
+        <v>10.0261430976688</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.06" customHeight="1">
@@ -2556,10 +2574,10 @@
         <v>111</v>
       </c>
       <c r="B113" s="14">
-        <v>59.4933767932454</v>
+        <v>58.2579344584315</v>
       </c>
       <c r="C113" s="15">
-        <v>9.2201841022857</v>
+        <v>10.7094687859766</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.06" customHeight="1">
@@ -2567,10 +2585,10 @@
         <v>112</v>
       </c>
       <c r="B114" s="11">
-        <v>60.8652444797895</v>
+        <v>57.4815636439715</v>
       </c>
       <c r="C114" s="12">
-        <v>8.997846852632</v>
+        <v>10.8641973805909</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.06" customHeight="1">
@@ -2578,10 +2596,10 @@
         <v>113</v>
       </c>
       <c r="B115" s="14">
-        <v>57.661745981658</v>
+        <v>57.5243123196594</v>
       </c>
       <c r="C115" s="15">
-        <v>9.7353830199998</v>
+        <v>10.3637108530843</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15.06" customHeight="1">
@@ -2589,10 +2607,10 @@
         <v>114</v>
       </c>
       <c r="B116" s="11">
-        <v>56.4312739371926</v>
+        <v>56.7335788557677</v>
       </c>
       <c r="C116" s="12">
-        <v>10.0793998294798</v>
+        <v>11.869993035915</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15.06" customHeight="1">
@@ -2600,10 +2618,10 @@
         <v>115</v>
       </c>
       <c r="B117" s="14">
-        <v>56.0037124340741</v>
+        <v>55.9507504385022</v>
       </c>
       <c r="C117" s="15">
-        <v>11.5403136677076</v>
+        <v>12.476696630348</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.06" customHeight="1">
@@ -2611,10 +2629,10 @@
         <v>116</v>
       </c>
       <c r="B118" s="11">
-        <v>56.0455361434544</v>
+        <v>58.5183522495253</v>
       </c>
       <c r="C118" s="12">
-        <v>10.9059268655567</v>
+        <v>9.8175710625056</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.06" customHeight="1">
@@ -2622,10 +2640,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="14">
-        <v>56.3925000060402</v>
+        <v>59.4933767932454</v>
       </c>
       <c r="C119" s="15">
-        <v>11.244290289142</v>
+        <v>9.2201841022857</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.06" customHeight="1">
@@ -2633,10 +2651,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="11">
-        <v>55.7500555765168</v>
+        <v>60.8652444797895</v>
       </c>
       <c r="C120" s="12">
-        <v>11.1895183685165</v>
+        <v>8.997846852632</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.06" customHeight="1">
@@ -2644,10 +2662,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="14">
-        <v>55.8109483708827</v>
+        <v>57.661745981658</v>
       </c>
       <c r="C121" s="15">
-        <v>10.8680885903786</v>
+        <v>9.7353830199998</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.06" customHeight="1">
@@ -2655,10 +2673,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="11">
-        <v>54.4190509838446</v>
+        <v>56.4312739371926</v>
       </c>
       <c r="C122" s="12">
-        <v>12.8625237125762</v>
+        <v>10.0793998294798</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.06" customHeight="1">
@@ -2666,10 +2684,10 @@
         <v>121</v>
       </c>
       <c r="B123" s="14">
-        <v>54.0745791774247</v>
+        <v>56.0037124340741</v>
       </c>
       <c r="C123" s="15">
-        <v>13.5561587706944</v>
+        <v>11.5403136677076</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.06" customHeight="1">
@@ -2677,10 +2695,10 @@
         <v>122</v>
       </c>
       <c r="B124" s="11">
-        <v>55.9262546765029</v>
+        <v>56.0455361434544</v>
       </c>
       <c r="C124" s="12">
-        <v>11.1200356326183</v>
+        <v>10.9059268655567</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.06" customHeight="1">
@@ -2688,10 +2706,10 @@
         <v>123</v>
       </c>
       <c r="B125" s="14">
-        <v>56.8207409261012</v>
+        <v>56.3925000060402</v>
       </c>
       <c r="C125" s="15">
-        <v>10.7923956439583</v>
+        <v>11.244290289142</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.06" customHeight="1">
@@ -2699,10 +2717,10 @@
         <v>124</v>
       </c>
       <c r="B126" s="11">
-        <v>57.3714461802261</v>
+        <v>55.7500555765168</v>
       </c>
       <c r="C126" s="12">
-        <v>10.1527591072801</v>
+        <v>11.1895183685165</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.06" customHeight="1">
@@ -2710,10 +2728,10 @@
         <v>125</v>
       </c>
       <c r="B127" s="14">
-        <v>56.6529777476856</v>
+        <v>55.8109483708827</v>
       </c>
       <c r="C127" s="15">
-        <v>10.5737807138864</v>
+        <v>10.8680885903786</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.06" customHeight="1">
@@ -2721,10 +2739,10 @@
         <v>126</v>
       </c>
       <c r="B128" s="11">
-        <v>55.5522853225424</v>
+        <v>54.4190509838446</v>
       </c>
       <c r="C128" s="12">
-        <v>11.1618695335786</v>
+        <v>12.8625237125762</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.06" customHeight="1">
@@ -2732,10 +2750,10 @@
         <v>127</v>
       </c>
       <c r="B129" s="14">
-        <v>54.6312310825228</v>
+        <v>54.0745791774247</v>
       </c>
       <c r="C129" s="15">
-        <v>12.684421983915</v>
+        <v>13.5561587706944</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.06" customHeight="1">
@@ -2743,10 +2761,10 @@
         <v>128</v>
       </c>
       <c r="B130" s="11">
-        <v>55.1525114915674</v>
+        <v>55.9262546765029</v>
       </c>
       <c r="C130" s="12">
-        <v>11.6356183368589</v>
+        <v>11.1200356326183</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15.06" customHeight="1">
@@ -2754,10 +2772,10 @@
         <v>129</v>
       </c>
       <c r="B131" s="14">
-        <v>54.8929007548477</v>
+        <v>56.8207409261012</v>
       </c>
       <c r="C131" s="15">
-        <v>12.0404335910972</v>
+        <v>10.7923956439583</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.06" customHeight="1">
@@ -2765,10 +2783,10 @@
         <v>130</v>
       </c>
       <c r="B132" s="11">
-        <v>55.4009241996912</v>
+        <v>57.3714461802261</v>
       </c>
       <c r="C132" s="12">
-        <v>12.2371286270183</v>
+        <v>10.1527591072801</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.06" customHeight="1">
@@ -2776,10 +2794,10 @@
         <v>131</v>
       </c>
       <c r="B133" s="14">
-        <v>54.2602260712253</v>
+        <v>56.6529777476856</v>
       </c>
       <c r="C133" s="15">
-        <v>11.8070467304142</v>
+        <v>10.5737807138864</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.06" customHeight="1">
@@ -2787,10 +2805,10 @@
         <v>132</v>
       </c>
       <c r="B134" s="11">
-        <v>54.5851131330458</v>
+        <v>55.5522853225424</v>
       </c>
       <c r="C134" s="12">
-        <v>12.5946001540522</v>
+        <v>11.1618695335786</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.06" customHeight="1">
@@ -2798,10 +2816,10 @@
         <v>133</v>
       </c>
       <c r="B135" s="14">
-        <v>53.0182229470343</v>
+        <v>54.6312310825228</v>
       </c>
       <c r="C135" s="15">
-        <v>14.6230779085162</v>
+        <v>12.684421983915</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.06" customHeight="1">
@@ -2809,10 +2827,10 @@
         <v>134</v>
       </c>
       <c r="B136" s="11">
-        <v>55.5003114889614</v>
+        <v>55.1525114915674</v>
       </c>
       <c r="C136" s="12">
-        <v>11.3114866850842</v>
+        <v>11.6356183368589</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.06" customHeight="1">
@@ -2820,10 +2838,10 @@
         <v>135</v>
       </c>
       <c r="B137" s="14">
-        <v>55.9246317527826</v>
+        <v>54.8929007548477</v>
       </c>
       <c r="C137" s="15">
-        <v>11.0783821431401</v>
+        <v>12.0404335910972</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.06" customHeight="1">
@@ -2831,10 +2849,10 @@
         <v>136</v>
       </c>
       <c r="B138" s="11">
-        <v>56.5531567950591</v>
+        <v>55.4009241996912</v>
       </c>
       <c r="C138" s="12">
-        <v>11.5455065211423</v>
+        <v>12.2371286270183</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15.06" customHeight="1">
@@ -2842,10 +2860,10 @@
         <v>137</v>
       </c>
       <c r="B139" s="14">
-        <v>53.3125249995886</v>
+        <v>54.2602260712253</v>
       </c>
       <c r="C139" s="15">
-        <v>12.1559626741874</v>
+        <v>11.8070467304142</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.06" customHeight="1">
@@ -2853,10 +2871,10 @@
         <v>138</v>
       </c>
       <c r="B140" s="11">
-        <v>53.3388512352356</v>
+        <v>54.5851131330458</v>
       </c>
       <c r="C140" s="12">
-        <v>11.7434568865306</v>
+        <v>12.5946001540522</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.06" customHeight="1">
@@ -2864,10 +2882,10 @@
         <v>139</v>
       </c>
       <c r="B141" s="14">
-        <v>53.8810871693838</v>
+        <v>53.0182229470343</v>
       </c>
       <c r="C141" s="15">
-        <v>12.6320611136098</v>
+        <v>14.6230779085162</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.06" customHeight="1">
@@ -2875,10 +2893,10 @@
         <v>140</v>
       </c>
       <c r="B142" s="11">
-        <v>54.2026659655414</v>
+        <v>55.5003114889614</v>
       </c>
       <c r="C142" s="12">
-        <v>11.3382380744366</v>
+        <v>11.3114866850842</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.06" customHeight="1">
@@ -2886,10 +2904,10 @@
         <v>141</v>
       </c>
       <c r="B143" s="14">
-        <v>54.4044092720515</v>
+        <v>55.9246317527826</v>
       </c>
       <c r="C143" s="15">
-        <v>11.6639081463958</v>
+        <v>11.0783821431401</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.06" customHeight="1">
@@ -2897,10 +2915,10 @@
         <v>142</v>
       </c>
       <c r="B144" s="11">
-        <v>54.0861621755935</v>
+        <v>56.5531567950591</v>
       </c>
       <c r="C144" s="12">
-        <v>12.1408216057158</v>
+        <v>11.5455065211423</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.06" customHeight="1">
@@ -2908,10 +2926,10 @@
         <v>143</v>
       </c>
       <c r="B145" s="14">
-        <v>53.3783095439168</v>
+        <v>53.3125249995886</v>
       </c>
       <c r="C145" s="15">
-        <v>11.9918620812419</v>
+        <v>12.1559626741874</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.06" customHeight="1">
@@ -2919,10 +2937,10 @@
         <v>144</v>
       </c>
       <c r="B146" s="11">
-        <v>52.1996002438094</v>
+        <v>53.3388512352356</v>
       </c>
       <c r="C146" s="12">
-        <v>12.4886022618426</v>
+        <v>11.7434568865306</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.06" customHeight="1">
@@ -2930,10 +2948,10 @@
         <v>145</v>
       </c>
       <c r="B147" s="14">
-        <v>50.3252901918307</v>
+        <v>53.8810871693838</v>
       </c>
       <c r="C147" s="15">
-        <v>14.2485790938621</v>
+        <v>12.6320611136098</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.06" customHeight="1">
@@ -2941,10 +2959,10 @@
         <v>146</v>
       </c>
       <c r="B148" s="11">
-        <v>52.2195992343542</v>
+        <v>54.2026659655414</v>
       </c>
       <c r="C148" s="12">
-        <v>10.6068081606259</v>
+        <v>11.3382380744366</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="15.06" customHeight="1">
@@ -2952,10 +2970,10 @@
         <v>147</v>
       </c>
       <c r="B149" s="14">
-        <v>51.3279666944708</v>
+        <v>54.4044092720515</v>
       </c>
       <c r="C149" s="15">
-        <v>10.8014453475453</v>
+        <v>11.6639081463958</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="15.06" customHeight="1">
@@ -2963,10 +2981,10 @@
         <v>148</v>
       </c>
       <c r="B150" s="11">
-        <v>52.7168895081709</v>
+        <v>54.0861621755935</v>
       </c>
       <c r="C150" s="12">
-        <v>10.1232272828135</v>
+        <v>12.1408216057158</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="15.06" customHeight="1">
@@ -2974,10 +2992,10 @@
         <v>149</v>
       </c>
       <c r="B151" s="14">
-        <v>52.1127351287154</v>
+        <v>53.3783095439168</v>
       </c>
       <c r="C151" s="15">
-        <v>10.9484225160804</v>
+        <v>11.9918620812419</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15.06" customHeight="1">
@@ -2985,10 +3003,10 @@
         <v>150</v>
       </c>
       <c r="B152" s="11">
-        <v>51.4793205045122</v>
+        <v>52.1996002438094</v>
       </c>
       <c r="C152" s="12">
-        <v>11.2159467785017</v>
+        <v>12.4886022618426</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="15.06" customHeight="1">
@@ -2996,10 +3014,10 @@
         <v>151</v>
       </c>
       <c r="B153" s="14">
-        <v>51.6134786204955</v>
+        <v>50.3252901918307</v>
       </c>
       <c r="C153" s="15">
-        <v>12.0638310422609</v>
+        <v>14.2485790938621</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.06" customHeight="1">
@@ -3007,10 +3025,10 @@
         <v>152</v>
       </c>
       <c r="B154" s="11">
-        <v>50.7779919402972</v>
+        <v>52.2195992343542</v>
       </c>
       <c r="C154" s="12">
-        <v>11.1724889657936</v>
+        <v>10.6068081606259</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.06" customHeight="1">
@@ -3018,10 +3036,10 @@
         <v>153</v>
       </c>
       <c r="B155" s="14">
-        <v>52.7432030166846</v>
+        <v>51.3279666944708</v>
       </c>
       <c r="C155" s="15">
-        <v>10.83821746076</v>
+        <v>10.8014453475453</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="15.06" customHeight="1">
@@ -3029,10 +3047,10 @@
         <v>154</v>
       </c>
       <c r="B156" s="11">
-        <v>52.9322826213147</v>
+        <v>52.7168895081709</v>
       </c>
       <c r="C156" s="12">
-        <v>11.1292562172452</v>
+        <v>10.1232272828135</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="15.06" customHeight="1">
@@ -3040,10 +3058,10 @@
         <v>155</v>
       </c>
       <c r="B157" s="14">
-        <v>53.002688346995</v>
+        <v>52.1127351287154</v>
       </c>
       <c r="C157" s="15">
-        <v>11.2245032398972</v>
+        <v>10.9484225160804</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="15.06" customHeight="1">
@@ -3051,10 +3069,10 @@
         <v>156</v>
       </c>
       <c r="B158" s="11">
-        <v>51.8991927647164</v>
+        <v>51.4793205045122</v>
       </c>
       <c r="C158" s="12">
-        <v>11.9854980801383</v>
+        <v>11.2159467785017</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="15.06" customHeight="1">
@@ -3062,10 +3080,10 @@
         <v>157</v>
       </c>
       <c r="B159" s="14">
-        <v>50.1302559190869</v>
+        <v>51.6134786204955</v>
       </c>
       <c r="C159" s="15">
-        <v>13.0790320816701</v>
+        <v>12.0638310422609</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="15.06" customHeight="1">
@@ -3073,10 +3091,10 @@
         <v>158</v>
       </c>
       <c r="B160" s="11">
-        <v>52.4302357833422</v>
+        <v>50.7779919402972</v>
       </c>
       <c r="C160" s="12">
-        <v>9.8938675934016</v>
+        <v>11.1724889657936</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.06" customHeight="1">
@@ -3084,10 +3102,10 @@
         <v>159</v>
       </c>
       <c r="B161" s="14">
-        <v>54.0557518257347</v>
+        <v>52.7432030166846</v>
       </c>
       <c r="C161" s="15">
-        <v>9.4157470723748</v>
+        <v>10.83821746076</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.06" customHeight="1">
@@ -3095,10 +3113,10 @@
         <v>160</v>
       </c>
       <c r="B162" s="11">
-        <v>54.5570824879941</v>
+        <v>52.9322826213147</v>
       </c>
       <c r="C162" s="12">
-        <v>10.0478539704553</v>
+        <v>11.1292562172452</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.06" customHeight="1">
@@ -3106,10 +3124,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="14">
-        <v>52.0676441315417</v>
+        <v>53.002688346995</v>
       </c>
       <c r="C163" s="15">
-        <v>10.8362757840182</v>
+        <v>11.2245032398972</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.06" customHeight="1">
@@ -3117,10 +3135,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="11">
-        <v>51.2622153772402</v>
+        <v>51.8991927647164</v>
       </c>
       <c r="C164" s="12">
-        <v>10.7313877375585</v>
+        <v>11.9854980801383</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.06" customHeight="1">
@@ -3128,10 +3146,10 @@
         <v>163</v>
       </c>
       <c r="B165" s="14">
-        <v>51.3397884953276</v>
+        <v>50.1302559190869</v>
       </c>
       <c r="C165" s="15">
-        <v>11.1595131185252</v>
+        <v>13.0790320816701</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15.06" customHeight="1">
@@ -3139,10 +3157,10 @@
         <v>164</v>
       </c>
       <c r="B166" s="11">
-        <v>51.5344661303082</v>
+        <v>52.4302357833422</v>
       </c>
       <c r="C166" s="12">
-        <v>11.1648311325302</v>
+        <v>9.8938675934016</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="15.06" customHeight="1">
@@ -3150,10 +3168,10 @@
         <v>165</v>
       </c>
       <c r="B167" s="14">
-        <v>51.0755943389931</v>
+        <v>54.0557518257347</v>
       </c>
       <c r="C167" s="15">
-        <v>11.5288657976635</v>
+        <v>9.4157470723748</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="15.06" customHeight="1">
@@ -3161,10 +3179,10 @@
         <v>166</v>
       </c>
       <c r="B168" s="11">
-        <v>52.2973468151966</v>
+        <v>54.5570824879941</v>
       </c>
       <c r="C168" s="12">
-        <v>10.9037708823633</v>
+        <v>10.0478539704553</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.06" customHeight="1">
@@ -3172,10 +3190,10 @@
         <v>167</v>
       </c>
       <c r="B169" s="14">
-        <v>50.425606177827</v>
+        <v>52.0676441315417</v>
       </c>
       <c r="C169" s="15">
-        <v>11.9274403618685</v>
+        <v>10.8362757840182</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="15.06" customHeight="1">
@@ -3183,10 +3201,10 @@
         <v>168</v>
       </c>
       <c r="B170" s="11">
-        <v>51.2134433404426</v>
+        <v>51.2622153772402</v>
       </c>
       <c r="C170" s="12">
-        <v>12.826173058498</v>
+        <v>10.7313877375585</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.06" customHeight="1">
@@ -3194,10 +3212,10 @@
         <v>169</v>
       </c>
       <c r="B171" s="14">
-        <v>48.9663052588155</v>
+        <v>51.3397884953276</v>
       </c>
       <c r="C171" s="15">
-        <v>13.8952967610189</v>
+        <v>11.1595131185252</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="15.06" customHeight="1">
@@ -3205,10 +3223,10 @@
         <v>170</v>
       </c>
       <c r="B172" s="11">
-        <v>50.8808363752997</v>
+        <v>51.5344661303082</v>
       </c>
       <c r="C172" s="12">
-        <v>11.7827545055176</v>
+        <v>11.1648311325302</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.06" customHeight="1">
@@ -3216,10 +3234,10 @@
         <v>171</v>
       </c>
       <c r="B173" s="14">
-        <v>50.822794440239</v>
+        <v>51.0755943389931</v>
       </c>
       <c r="C173" s="15">
-        <v>10.9381318843905</v>
+        <v>11.5288657976635</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="15.06" customHeight="1">
@@ -3227,10 +3245,10 @@
         <v>172</v>
       </c>
       <c r="B174" s="11">
-        <v>51.2041056812479</v>
+        <v>52.2973468151966</v>
       </c>
       <c r="C174" s="12">
-        <v>11.3547264160474</v>
+        <v>10.9037708823633</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="15.06" customHeight="1">
@@ -3238,10 +3256,10 @@
         <v>173</v>
       </c>
       <c r="B175" s="14">
-        <v>49.9854714193123</v>
+        <v>50.425606177827</v>
       </c>
       <c r="C175" s="15">
-        <v>12.890167075463</v>
+        <v>11.9274403618685</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="15.06" customHeight="1">
@@ -3249,10 +3267,10 @@
         <v>174</v>
       </c>
       <c r="B176" s="11">
-        <v>50.8720560696387</v>
+        <v>51.2134433404426</v>
       </c>
       <c r="C176" s="12">
-        <v>12.7922191898613</v>
+        <v>12.826173058498</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15.06" customHeight="1">
@@ -3260,10 +3278,10 @@
         <v>175</v>
       </c>
       <c r="B177" s="14">
-        <v>52.8570656404413</v>
+        <v>48.9663052588155</v>
       </c>
       <c r="C177" s="15">
-        <v>12.3891350076662</v>
+        <v>13.8952967610189</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="15.06" customHeight="1">
@@ -3271,10 +3289,10 @@
         <v>176</v>
       </c>
       <c r="B178" s="11">
-        <v>54.2348904667938</v>
+        <v>50.8808363752997</v>
       </c>
       <c r="C178" s="12">
-        <v>10.6070967020237</v>
+        <v>11.7827545055176</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="15.06" customHeight="1">
@@ -3282,10 +3300,10 @@
         <v>177</v>
       </c>
       <c r="B179" s="14">
-        <v>52.6717218134372</v>
+        <v>50.822794440239</v>
       </c>
       <c r="C179" s="15">
-        <v>11.8836844308216</v>
+        <v>10.9381318843905</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="15.06" customHeight="1">
@@ -3293,10 +3311,10 @@
         <v>178</v>
       </c>
       <c r="B180" s="11">
-        <v>52.0620341684202</v>
+        <v>51.2041056812479</v>
       </c>
       <c r="C180" s="12">
-        <v>12.0098894209605</v>
+        <v>11.3547264160474</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="15.06" customHeight="1">
@@ -3304,10 +3322,10 @@
         <v>179</v>
       </c>
       <c r="B181" s="14">
-        <v>53.9570404750343</v>
+        <v>49.9854714193123</v>
       </c>
       <c r="C181" s="15">
-        <v>11.3440989290337</v>
+        <v>12.890167075463</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="15.06" customHeight="1">
@@ -3315,10 +3333,10 @@
         <v>180</v>
       </c>
       <c r="B182" s="11">
-        <v>52.5582801429711</v>
+        <v>50.8720560696387</v>
       </c>
       <c r="C182" s="12">
-        <v>12.9996017411798</v>
+        <v>12.7922191898613</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="15.06" customHeight="1">
@@ -3326,10 +3344,10 @@
         <v>181</v>
       </c>
       <c r="B183" s="14">
-        <v>52.054783513384</v>
+        <v>52.8570656404413</v>
       </c>
       <c r="C183" s="15">
-        <v>13.4084601825721</v>
+        <v>12.3891350076662</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="15.06" customHeight="1">
@@ -3337,10 +3355,10 @@
         <v>182</v>
       </c>
       <c r="B184" s="11">
-        <v>55.1613835658971</v>
+        <v>54.2348904667938</v>
       </c>
       <c r="C184" s="12">
-        <v>10.3343851862214</v>
+        <v>10.6070967020237</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="15.06" customHeight="1">
@@ -3348,10 +3366,10 @@
         <v>183</v>
       </c>
       <c r="B185" s="14">
-        <v>54.6923619604569</v>
+        <v>52.6717218134372</v>
       </c>
       <c r="C185" s="15">
-        <v>10.207395984046</v>
+        <v>11.8836844308216</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="15.06" customHeight="1">
@@ -3359,10 +3377,10 @@
         <v>184</v>
       </c>
       <c r="B186" s="11">
-        <v>55.4219747676188</v>
+        <v>52.0620341684202</v>
       </c>
       <c r="C186" s="12">
-        <v>9.9550118079072</v>
+        <v>12.0098894209605</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="15.06" customHeight="1">
@@ -3370,10 +3388,10 @@
         <v>185</v>
       </c>
       <c r="B187" s="14">
-        <v>53.6798234688621</v>
+        <v>53.9570404750343</v>
       </c>
       <c r="C187" s="15">
-        <v>11.1717549024796</v>
+        <v>11.3440989290337</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="15.06" customHeight="1">
@@ -3381,10 +3399,10 @@
         <v>186</v>
       </c>
       <c r="B188" s="11">
-        <v>53.0556257598427</v>
+        <v>52.5582801429711</v>
       </c>
       <c r="C188" s="12">
-        <v>11.7543799111374</v>
+        <v>12.9996017411798</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="15.06" customHeight="1">
@@ -3392,10 +3410,10 @@
         <v>187</v>
       </c>
       <c r="B189" s="14">
-        <v>54.0537573997119</v>
+        <v>52.054783513384</v>
       </c>
       <c r="C189" s="15">
-        <v>11.9960860877311</v>
+        <v>13.4084601825721</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="15.06" customHeight="1">
@@ -3403,10 +3421,10 @@
         <v>188</v>
       </c>
       <c r="B190" s="11">
-        <v>52.5215285529539</v>
+        <v>55.1613835658971</v>
       </c>
       <c r="C190" s="12">
-        <v>11.5232939285148</v>
+        <v>10.3343851862214</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="15.06" customHeight="1">
@@ -3414,10 +3432,10 @@
         <v>189</v>
       </c>
       <c r="B191" s="14">
-        <v>52.8468099310153</v>
+        <v>54.6923619604569</v>
       </c>
       <c r="C191" s="15">
-        <v>12.3053981642655</v>
+        <v>10.207395984046</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="15.06" customHeight="1">
@@ -3425,10 +3443,10 @@
         <v>190</v>
       </c>
       <c r="B192" s="11">
-        <v>52.8372655355322</v>
+        <v>55.4219747676188</v>
       </c>
       <c r="C192" s="12">
-        <v>12.0611506304217</v>
+        <v>9.9550118079072</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="15.06" customHeight="1">
@@ -3436,10 +3454,10 @@
         <v>191</v>
       </c>
       <c r="B193" s="14">
-        <v>52.1961450641635</v>
+        <v>53.6798234688621</v>
       </c>
       <c r="C193" s="15">
-        <v>12.9483637679849</v>
+        <v>11.1717549024796</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="15.06" customHeight="1">
@@ -3447,10 +3465,10 @@
         <v>192</v>
       </c>
       <c r="B194" s="11">
-        <v>51.6887178546969</v>
+        <v>53.0556257598427</v>
       </c>
       <c r="C194" s="12">
-        <v>14.2292142828116</v>
+        <v>11.7543799111374</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="15.06" customHeight="1">
@@ -3458,10 +3476,10 @@
         <v>193</v>
       </c>
       <c r="B195" s="14">
-        <v>52.3867318474328</v>
+        <v>54.0537573997119</v>
       </c>
       <c r="C195" s="15">
-        <v>13.2183132733731</v>
+        <v>11.9960860877311</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="15.06" customHeight="1">
@@ -3469,10 +3487,10 @@
         <v>194</v>
       </c>
       <c r="B196" s="11">
-        <v>53.5557014794664</v>
+        <v>52.5215285529539</v>
       </c>
       <c r="C196" s="12">
-        <v>12.0707434505172</v>
+        <v>11.5232939285148</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="15.06" customHeight="1">
@@ -3480,10 +3498,10 @@
         <v>195</v>
       </c>
       <c r="B197" s="14">
-        <v>54.3961586863965</v>
+        <v>52.8468099310153</v>
       </c>
       <c r="C197" s="15">
-        <v>11.7769742339699</v>
+        <v>12.3053981642655</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="15.06" customHeight="1">
@@ -3491,10 +3509,10 @@
         <v>196</v>
       </c>
       <c r="B198" s="11">
-        <v>53.7983147515861</v>
+        <v>52.8372655355322</v>
       </c>
       <c r="C198" s="12">
-        <v>12.5941851468136</v>
+        <v>12.0611506304217</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="15.06" customHeight="1">
@@ -3502,10 +3520,10 @@
         <v>197</v>
       </c>
       <c r="B199" s="14">
-        <v>53.0643998711001</v>
+        <v>52.1961450641635</v>
       </c>
       <c r="C199" s="15">
-        <v>12.5146666412604</v>
+        <v>12.9483637679849</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="15.06" customHeight="1">
@@ -3513,10 +3531,10 @@
         <v>198</v>
       </c>
       <c r="B200" s="11">
-        <v>52.7672828458545</v>
+        <v>51.6887178546969</v>
       </c>
       <c r="C200" s="12">
-        <v>13.0851112362465</v>
+        <v>14.2292142828116</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="15.06" customHeight="1">
@@ -3524,10 +3542,10 @@
         <v>199</v>
       </c>
       <c r="B201" s="14">
-        <v>53.5209970424871</v>
+        <v>52.3867318474328</v>
       </c>
       <c r="C201" s="15">
-        <v>12.9400443620063</v>
+        <v>13.2183132733731</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="15.06" customHeight="1">
@@ -3535,10 +3553,10 @@
         <v>200</v>
       </c>
       <c r="B202" s="11">
-        <v>51.5936901371508</v>
+        <v>53.5557014794664</v>
       </c>
       <c r="C202" s="12">
-        <v>13.9956895410496</v>
+        <v>12.0707434505172</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="15.06" customHeight="1">
@@ -3546,10 +3564,10 @@
         <v>201</v>
       </c>
       <c r="B203" s="14">
-        <v>53.1164704158262</v>
+        <v>54.3961586863965</v>
       </c>
       <c r="C203" s="15">
-        <v>13.7523369037492</v>
+        <v>11.7769742339699</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="15.06" customHeight="1">
@@ -3557,10 +3575,10 @@
         <v>202</v>
       </c>
       <c r="B204" s="11">
-        <v>52.6944602755838</v>
+        <v>53.7983147515861</v>
       </c>
       <c r="C204" s="12">
-        <v>14.6770965923023</v>
+        <v>12.5941851468136</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="15.06" customHeight="1">
@@ -3568,10 +3586,10 @@
         <v>203</v>
       </c>
       <c r="B205" s="14">
-        <v>53.705275422389</v>
+        <v>53.0643998711001</v>
       </c>
       <c r="C205" s="15">
-        <v>13.6238377743265</v>
+        <v>12.5146666412604</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="15.06" customHeight="1">
@@ -3579,10 +3597,10 @@
         <v>204</v>
       </c>
       <c r="B206" s="11">
-        <v>52.5295688876554</v>
+        <v>52.7672828458545</v>
       </c>
       <c r="C206" s="12">
-        <v>15.6875978111418</v>
+        <v>13.0851112362465</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="15.06" customHeight="1">
@@ -3590,10 +3608,10 @@
         <v>205</v>
       </c>
       <c r="B207" s="14">
-        <v>52.1300389423391</v>
+        <v>53.5209970424871</v>
       </c>
       <c r="C207" s="15">
-        <v>17.0030725069589</v>
+        <v>12.9400443620063</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="15.06" customHeight="1">
@@ -3601,10 +3619,10 @@
         <v>206</v>
       </c>
       <c r="B208" s="11">
-        <v>55.2255491401209</v>
+        <v>51.5936901371508</v>
       </c>
       <c r="C208" s="12">
-        <v>12.185562128385</v>
+        <v>13.9956895410496</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="15.06" customHeight="1">
@@ -3612,10 +3630,10 @@
         <v>207</v>
       </c>
       <c r="B209" s="14">
-        <v>55.5763482052239</v>
+        <v>53.1164704158262</v>
       </c>
       <c r="C209" s="15">
-        <v>12.911682543941</v>
+        <v>13.7523369037492</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="15.06" customHeight="1">
@@ -3623,10 +3641,10 @@
         <v>208</v>
       </c>
       <c r="B210" s="11">
-        <v>55.4974585013471</v>
+        <v>52.6944602755838</v>
       </c>
       <c r="C210" s="12">
-        <v>13.700866564958</v>
+        <v>14.6770965923023</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="15.06" customHeight="1">
@@ -3634,10 +3652,10 @@
         <v>209</v>
       </c>
       <c r="B211" s="14">
-        <v>54.2846369587918</v>
+        <v>53.705275422389</v>
       </c>
       <c r="C211" s="15">
-        <v>14.2587874366084</v>
+        <v>13.6238377743265</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="15.06" customHeight="1">
@@ -3645,10 +3663,10 @@
         <v>210</v>
       </c>
       <c r="B212" s="11">
-        <v>54.1432207443421</v>
+        <v>52.5295688876554</v>
       </c>
       <c r="C212" s="12">
-        <v>14.4335823745174</v>
+        <v>15.6875978111418</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="15.06" customHeight="1">
@@ -3656,10 +3674,10 @@
         <v>211</v>
       </c>
       <c r="B213" s="14">
-        <v>52.9678975168235</v>
+        <v>52.1300389423391</v>
       </c>
       <c r="C213" s="15">
-        <v>14.4433640728583</v>
+        <v>17.0030725069589</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="15.06" customHeight="1">
@@ -3667,10 +3685,10 @@
         <v>212</v>
       </c>
       <c r="B214" s="11">
-        <v>52.5348575015193</v>
+        <v>55.2255491401209</v>
       </c>
       <c r="C214" s="12">
-        <v>14.1356808126726</v>
+        <v>12.185562128385</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15.06" customHeight="1">
@@ -3678,10 +3696,10 @@
         <v>213</v>
       </c>
       <c r="B215" s="14">
-        <v>54.8945382052825</v>
+        <v>55.5763482052239</v>
       </c>
       <c r="C215" s="15">
-        <v>12.8930250407356</v>
+        <v>12.911682543941</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="15.06" customHeight="1">
@@ -3689,10 +3707,10 @@
         <v>214</v>
       </c>
       <c r="B216" s="11">
-        <v>53.3478279506793</v>
+        <v>55.4974585013471</v>
       </c>
       <c r="C216" s="12">
-        <v>14.8011528253016</v>
+        <v>13.700866564958</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="15.06" customHeight="1">
@@ -3700,10 +3718,10 @@
         <v>215</v>
       </c>
       <c r="B217" s="14">
-        <v>54.4659239265533</v>
+        <v>54.2846369587918</v>
       </c>
       <c r="C217" s="15">
-        <v>12.9835218184633</v>
+        <v>14.2587874366084</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="15.06" customHeight="1">
@@ -3711,10 +3729,10 @@
         <v>216</v>
       </c>
       <c r="B218" s="11">
-        <v>52.5686988424649</v>
+        <v>54.1432207443421</v>
       </c>
       <c r="C218" s="12">
-        <v>16.2819491475553</v>
+        <v>14.4335823745174</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="15.06" customHeight="1">
@@ -3722,10 +3740,10 @@
         <v>217</v>
       </c>
       <c r="B219" s="14">
-        <v>51.9537460676232</v>
+        <v>52.9678975168235</v>
       </c>
       <c r="C219" s="15">
-        <v>16.1150787533156</v>
+        <v>14.4433640728583</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.06" customHeight="1">
@@ -3733,10 +3751,10 @@
         <v>218</v>
       </c>
       <c r="B220" s="11">
-        <v>52.2396211413925</v>
+        <v>52.5348575015193</v>
       </c>
       <c r="C220" s="12">
-        <v>15.7729772045571</v>
+        <v>14.1356808126726</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="15.06" customHeight="1">
@@ -3744,10 +3762,10 @@
         <v>219</v>
       </c>
       <c r="B221" s="14">
-        <v>53.669361375132</v>
+        <v>54.8945382052825</v>
       </c>
       <c r="C221" s="15">
-        <v>14.7076154416823</v>
+        <v>12.8930250407356</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="15.06" customHeight="1">
@@ -3755,10 +3773,10 @@
         <v>220</v>
       </c>
       <c r="B222" s="11">
-        <v>53.8657748353357</v>
+        <v>53.3478279506793</v>
       </c>
       <c r="C222" s="12">
-        <v>14.8087640920827</v>
+        <v>14.8011528253016</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="15.06" customHeight="1">
@@ -3766,10 +3784,10 @@
         <v>221</v>
       </c>
       <c r="B223" s="14">
-        <v>52.1849773909506</v>
+        <v>54.4659239265533</v>
       </c>
       <c r="C223" s="15">
-        <v>14.5554557092204</v>
+        <v>12.9835218184633</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.06" customHeight="1">
@@ -3777,10 +3795,10 @@
         <v>222</v>
       </c>
       <c r="B224" s="11">
-        <v>51.6010895397791</v>
+        <v>52.5686988424649</v>
       </c>
       <c r="C224" s="12">
-        <v>15.7841747353288</v>
+        <v>16.2819491475553</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="15.06" customHeight="1">
@@ -3788,10 +3806,10 @@
         <v>223</v>
       </c>
       <c r="B225" s="14">
-        <v>52.7926451068711</v>
+        <v>51.9537460676232</v>
       </c>
       <c r="C225" s="15">
-        <v>15.4082957005055</v>
+        <v>16.1150787533156</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="15.06" customHeight="1">
@@ -3799,10 +3817,10 @@
         <v>224</v>
       </c>
       <c r="B226" s="11">
-        <v>51.3252581877848</v>
+        <v>52.2396211413925</v>
       </c>
       <c r="C226" s="12">
-        <v>16.2525328891098</v>
+        <v>15.7729772045571</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="15.06" customHeight="1">
@@ -3810,10 +3828,10 @@
         <v>225</v>
       </c>
       <c r="B227" s="14">
-        <v>53.0179942612247</v>
+        <v>53.669361375132</v>
       </c>
       <c r="C227" s="15">
-        <v>14.4253500471206</v>
+        <v>14.7076154416823</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="15.06" customHeight="1">
@@ -3821,10 +3839,10 @@
         <v>226</v>
       </c>
       <c r="B228" s="11">
-        <v>52.6011807280768</v>
+        <v>53.8657748353357</v>
       </c>
       <c r="C228" s="12">
-        <v>16.2876752580982</v>
+        <v>14.8087640920827</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="15.06" customHeight="1">
@@ -3832,10 +3850,10 @@
         <v>227</v>
       </c>
       <c r="B229" s="14">
-        <v>52.5499876394901</v>
+        <v>52.1849773909506</v>
       </c>
       <c r="C229" s="15">
-        <v>14.9539159319882</v>
+        <v>14.5554557092204</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="15.06" customHeight="1">
@@ -3843,10 +3861,10 @@
         <v>228</v>
       </c>
       <c r="B230" s="11">
-        <v>52.7217813211204</v>
+        <v>51.6010895397791</v>
       </c>
       <c r="C230" s="12">
-        <v>15.854205519729</v>
+        <v>15.7841747353288</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="15.06" customHeight="1">
@@ -3854,10 +3872,10 @@
         <v>229</v>
       </c>
       <c r="B231" s="14">
-        <v>52.1922832429617</v>
+        <v>52.7926451068711</v>
       </c>
       <c r="C231" s="15">
-        <v>17.8727135286198</v>
+        <v>15.4082957005055</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="15.06" customHeight="1">
@@ -3865,10 +3883,10 @@
         <v>230</v>
       </c>
       <c r="B232" s="11">
-        <v>55.2331527848448</v>
+        <v>51.3252581877848</v>
       </c>
       <c r="C232" s="12">
-        <v>13.8393172072269</v>
+        <v>16.2525328891098</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="15.06" customHeight="1">
@@ -3876,10 +3894,10 @@
         <v>231</v>
       </c>
       <c r="B233" s="14">
-        <v>55.9261540946299</v>
+        <v>53.0179942612247</v>
       </c>
       <c r="C233" s="15">
-        <v>13.5516310144914</v>
+        <v>14.4253500471206</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="15.06" customHeight="1">
@@ -3887,10 +3905,10 @@
         <v>232</v>
       </c>
       <c r="B234" s="11">
-        <v>53.8128262040342</v>
+        <v>52.6011807280768</v>
       </c>
       <c r="C234" s="12">
-        <v>14.5854832832329</v>
+        <v>16.2876752580982</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="15.06" customHeight="1">
@@ -3898,10 +3916,10 @@
         <v>233</v>
       </c>
       <c r="B235" s="14">
-        <v>53.8776073722885</v>
+        <v>52.5499876394901</v>
       </c>
       <c r="C235" s="15">
-        <v>14.280508224643</v>
+        <v>14.9539159319882</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="15.06" customHeight="1">
@@ -3909,10 +3927,10 @@
         <v>234</v>
       </c>
       <c r="B236" s="11">
-        <v>52.9378525078841</v>
+        <v>52.7217813211204</v>
       </c>
       <c r="C236" s="12">
-        <v>14.7076367570061</v>
+        <v>15.854205519729</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="15.06" customHeight="1">
@@ -3920,10 +3938,10 @@
         <v>235</v>
       </c>
       <c r="B237" s="14">
-        <v>52.0959255184382</v>
+        <v>52.1922832429617</v>
       </c>
       <c r="C237" s="15">
-        <v>15.0219078528999</v>
+        <v>17.8727135286198</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="15.06" customHeight="1">
@@ -3931,10 +3949,10 @@
         <v>236</v>
       </c>
       <c r="B238" s="11">
-        <v>51.7606877803257</v>
+        <v>55.2331527848448</v>
       </c>
       <c r="C238" s="12">
-        <v>15.2320441726882</v>
+        <v>13.8393172072269</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="15.06" customHeight="1">
@@ -3942,10 +3960,10 @@
         <v>237</v>
       </c>
       <c r="B239" s="14">
-        <v>51.2329807591797</v>
+        <v>55.9261540946299</v>
       </c>
       <c r="C239" s="15">
-        <v>14.2262985847995</v>
+        <v>13.5516310144914</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="15.06" customHeight="1">
@@ -3953,10 +3971,10 @@
         <v>238</v>
       </c>
       <c r="B240" s="11">
-        <v>51.4545320954634</v>
+        <v>53.8128262040342</v>
       </c>
       <c r="C240" s="12">
-        <v>14.5898642664963</v>
+        <v>14.5854832832329</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.06" customHeight="1">
@@ -3964,10 +3982,10 @@
         <v>239</v>
       </c>
       <c r="B241" s="14">
-        <v>53.0179193342885</v>
+        <v>53.8776073722885</v>
       </c>
       <c r="C241" s="15">
-        <v>15.7050562411223</v>
+        <v>14.280508224643</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="15.06" customHeight="1">
@@ -3975,10 +3993,10 @@
         <v>240</v>
       </c>
       <c r="B242" s="11">
-        <v>52.7136795701075</v>
+        <v>52.9378525078841</v>
       </c>
       <c r="C242" s="12">
-        <v>17.3070228644639</v>
+        <v>14.7076367570061</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="15.06" customHeight="1">
@@ -3986,112 +4004,130 @@
         <v>241</v>
       </c>
       <c r="B243" s="14">
+        <v>52.0959255184382</v>
+      </c>
+      <c r="C243" s="15">
+        <v>15.0219078528999</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A244" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B244" s="11">
+        <v>51.7606877803257</v>
+      </c>
+      <c r="C244" s="12">
+        <v>15.2320441726882</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A245" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B245" s="14">
+        <v>51.2329807591797</v>
+      </c>
+      <c r="C245" s="15">
+        <v>14.2262985847995</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A246" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B246" s="11">
+        <v>51.4545320954634</v>
+      </c>
+      <c r="C246" s="12">
+        <v>14.5898642664963</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A247" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B247" s="14">
+        <v>53.0179193342885</v>
+      </c>
+      <c r="C247" s="15">
+        <v>15.7050562411223</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A248" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B248" s="11">
+        <v>52.7136795701075</v>
+      </c>
+      <c r="C248" s="12">
+        <v>17.3070228644639</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="15.06" customHeight="1">
+      <c r="A249" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B249" s="14">
         <v>53.008759880627</v>
       </c>
-      <c r="C243" s="15">
+      <c r="C249" s="15">
         <v>16.6946796667751</v>
       </c>
     </row>
-    <row r="244" spans="1:1">
-      <c r="A244" s="3" t="s">
+    <row r="250" spans="1:1">
+      <c r="A250" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
-      <c r="A245" s="16" t="s">
+    <row r="251" spans="1:4">
+      <c r="A251" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B245" s="16"/>
-      <c r="C245" s="16"/>
-      <c r="D245" s="16"/>
-    </row>
-    <row r="246" spans="1:4">
-      <c r="A246" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="B246" s="17"/>
-      <c r="C246" s="17"/>
-      <c r="D246" s="17"/>
-    </row>
-    <row r="247" spans="1:4">
-      <c r="A247" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="B247" s="18"/>
-      <c r="C247" s="18"/>
-      <c r="D247" s="18"/>
-    </row>
-    <row r="248" spans="1:4">
-      <c r="A248" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="B248" s="18"/>
-      <c r="C248" s="18"/>
-      <c r="D248" s="18"/>
-    </row>
-    <row r="249" spans="1:4">
-      <c r="A249" s="18" t="s">
+      <c r="B251" s="16"/>
+      <c r="C251" s="16"/>
+      <c r="D251" s="16"/>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B252" s="17"/>
+      <c r="C252" s="17"/>
+      <c r="D252" s="17"/>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B253" s="18"/>
+      <c r="C253" s="18"/>
+      <c r="D253" s="18"/>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B254" s="18"/>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B249" s="18"/>
-      <c r="C249" s="18"/>
-      <c r="D249" s="18"/>
-    </row>
-    <row r="250" spans="1:4">
-      <c r="A250" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="B250" s="18"/>
-      <c r="C250" s="18"/>
-      <c r="D250" s="18"/>
-    </row>
-    <row r="251" spans="1:4">
-      <c r="A251" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="B251" s="19"/>
-      <c r="C251" s="19"/>
-      <c r="D251" s="19"/>
-    </row>
-    <row r="252" spans="1:4">
-      <c r="A252" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="B252" s="19"/>
-      <c r="C252" s="19"/>
-      <c r="D252" s="19"/>
-    </row>
-    <row r="253" spans="1:4">
-      <c r="A253" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="B253" s="19"/>
-      <c r="C253" s="19"/>
-      <c r="D253" s="19"/>
-    </row>
-    <row r="254" spans="1:4">
-      <c r="A254" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="B254" s="19"/>
-      <c r="C254" s="19"/>
-      <c r="D254" s="19"/>
-    </row>
-    <row r="255" spans="1:4">
-      <c r="A255" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="B255" s="19"/>
-      <c r="C255" s="19"/>
-      <c r="D255" s="19"/>
+      <c r="B255" s="18"/>
+      <c r="C255" s="18"/>
+      <c r="D255" s="18"/>
     </row>
     <row r="256" spans="1:4">
-      <c r="A256" s="19" t="s">
+      <c r="A256" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="B256" s="19"/>
-      <c r="C256" s="19"/>
-      <c r="D256" s="19"/>
+      <c r="B256" s="18"/>
+      <c r="C256" s="18"/>
+      <c r="D256" s="18"/>
     </row>
     <row r="257" spans="1:4">
       <c r="A257" s="19" t="s">
@@ -4117,29 +4153,77 @@
       <c r="C259" s="19"/>
       <c r="D259" s="19"/>
     </row>
-    <row r="260" spans="1:1">
-      <c r="A260" s="20" t="s">
+    <row r="260" spans="1:4">
+      <c r="A260" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B260" s="19"/>
+      <c r="C260" s="19"/>
+      <c r="D260" s="19"/>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B261" s="19"/>
+      <c r="C261" s="19"/>
+      <c r="D261" s="19"/>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B262" s="19"/>
+      <c r="C262" s="19"/>
+      <c r="D262" s="19"/>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B263" s="19"/>
+      <c r="C263" s="19"/>
+      <c r="D263" s="19"/>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B264" s="19"/>
+      <c r="C264" s="19"/>
+      <c r="D264" s="19"/>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B265" s="19"/>
+      <c r="C265" s="19"/>
+      <c r="D265" s="19"/>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
-      <c r="A261" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="B261" s="21"/>
-      <c r="C261" s="21"/>
-      <c r="D261" s="21"/>
-    </row>
-    <row r="262" spans="1:4">
-      <c r="A262" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="B262" s="21"/>
-      <c r="C262" s="21"/>
-      <c r="D262" s="21"/>
-    </row>
-    <row r="263" spans="1:1">
-      <c r="A263" s="22" t="s">
+    <row r="267" spans="1:4">
+      <c r="A267" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="B267" s="21"/>
+      <c r="C267" s="21"/>
+      <c r="D267" s="21"/>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="B268" s="21"/>
+      <c r="C268" s="21"/>
+      <c r="D268" s="21"/>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" s="22" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4147,12 +4231,6 @@
   <mergeCells count="19">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A246:D246"/>
-    <mergeCell ref="A247:D247"/>
-    <mergeCell ref="A248:D248"/>
-    <mergeCell ref="A249:D249"/>
-    <mergeCell ref="A250:D250"/>
     <mergeCell ref="A251:D251"/>
     <mergeCell ref="A252:D252"/>
     <mergeCell ref="A253:D253"/>
@@ -4162,11 +4240,17 @@
     <mergeCell ref="A257:D257"/>
     <mergeCell ref="A258:D258"/>
     <mergeCell ref="A259:D259"/>
+    <mergeCell ref="A260:D260"/>
     <mergeCell ref="A261:D261"/>
     <mergeCell ref="A262:D262"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A264:D264"/>
+    <mergeCell ref="A265:D265"/>
+    <mergeCell ref="A267:D267"/>
+    <mergeCell ref="A268:D268"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A248" r:id="rId1"/>
+    <hyperlink ref="A254" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>